<commit_message>
add last update message.
</commit_message>
<xml_diff>
--- a/extras/sample-form/display-graph_sample_form.xlsx
+++ b/extras/sample-form/display-graph_sample_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\display-graph\extras\sample-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B036FE2F-DFAD-4A88-9210-5698515BE4D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A768F5-5926-4487-90D7-05A12620FF2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5220,7 +5220,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -6047,7 +6047,7 @@
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2008121213</v>
+        <v>2008121739</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>

</xml_diff>